<commit_message>
validation chap 7 extraction
</commit_message>
<xml_diff>
--- a/code/outputs/P1_summary_true_table.xlsx
+++ b/code/outputs/P1_summary_true_table.xlsx
@@ -49,7 +49,7 @@
     <t>§ 275.0-7_P1</t>
   </si>
   <si>
-    <t>p1_true_table.json</t>
+    <t>documents_true_table.json</t>
   </si>
 </sst>
 </file>
@@ -453,13 +453,13 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>21</v>
       </c>
       <c r="G2">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -479,13 +479,13 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <v>12</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>

</xml_diff>